<commit_message>
No ratio replacement updated - 20170522
</commit_message>
<xml_diff>
--- a/static/matrices/Credit Ascent Primary Matrix.xlsx
+++ b/static/matrices/Credit Ascent Primary Matrix.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rwulbern\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Walker\Web Pricer\matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Credit Ascent-Primary" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="129">
   <si>
     <t>Credit Ascent - Primary Residence</t>
   </si>
@@ -317,9 +317,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">     Fully-Indexed Rate or Note Rate + Initial Cap (2%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">     Fully-Indexed Rate or Note Rate</t>
   </si>
   <si>
@@ -329,10 +326,10 @@
     <t xml:space="preserve">  • Floor = Margin</t>
   </si>
   <si>
-    <t xml:space="preserve">  • Margin (A, A- Grades): 5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  • Margin (B+,B,B-,C Grades): 6%</t>
+    <t xml:space="preserve">  • Margin (A, A- Grades): 4.5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  • Margin (B+,B,B-,C Grades): 5.5%</t>
   </si>
   <si>
     <t>Interest Only</t>
@@ -472,10 +469,10 @@
     <t xml:space="preserve">                        ◦ A, A-, &amp; B+ Grade Only</t>
   </si>
   <si>
-    <t>Eligibile States</t>
-  </si>
-  <si>
-    <t>Nationwide excluding Puerto Rico, Guam and the US Virgin Islands; DC, MD, NJ and NY restricted to a 660 minimum FICO w/ a max LTV/CLTV of 80%</t>
+    <t>Eligible States</t>
+  </si>
+  <si>
+    <t>Nationwide excluding Puerto Rico, Guam and the US Virgin Islands; DC, MD, NJ and NY restricted to a 660 minimum FICO w/ a max LTV/CLTV of 85%</t>
   </si>
   <si>
     <t>Escrows:</t>
@@ -487,7 +484,7 @@
     <t>Points and Fees:</t>
   </si>
   <si>
-    <t>May not exceed 3%</t>
+    <t>May not exceed 5%</t>
   </si>
   <si>
     <t>Interested Party Contribution:</t>
@@ -729,7 +726,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -766,6 +763,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="58">
     <border>
@@ -1504,7 +1507,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="247">
+  <cellXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1944,25 +1947,34 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -2029,6 +2041,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2038,16 +2053,19 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2080,7 +2098,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2504,10 +2522,10 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="5" topLeftCell="F53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D83" sqref="D83"/>
+      <selection pane="bottomRight" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,7 +2548,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="3">
-        <v>42681</v>
+        <v>42856</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3649,24 +3667,24 @@
       <c r="C56" s="146"/>
       <c r="D56" s="147"/>
       <c r="E56" s="148" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F56" s="146"/>
       <c r="G56" s="149"/>
       <c r="H56" s="150" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I56" s="151"/>
     </row>
     <row r="57" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="144"/>
       <c r="B57" s="145" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C57" s="152"/>
       <c r="D57" s="153"/>
       <c r="E57" s="153" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F57" s="154"/>
       <c r="G57" s="149"/>
@@ -3676,353 +3694,353 @@
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="144"/>
       <c r="B58" s="155" t="s">
-        <v>83</v>
-      </c>
-      <c r="C58" s="152"/>
+        <v>82</v>
+      </c>
+      <c r="C58" s="156"/>
       <c r="D58" s="153"/>
-      <c r="E58" s="153" t="s">
-        <v>83</v>
-      </c>
-      <c r="F58" s="156"/>
+      <c r="E58" s="157" t="s">
+        <v>82</v>
+      </c>
+      <c r="F58" s="158"/>
       <c r="G58" s="149"/>
       <c r="H58" s="149"/>
-      <c r="I58" s="157"/>
+      <c r="I58" s="159"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="144"/>
-      <c r="B59" s="158" t="s">
+      <c r="B59" s="160" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="161"/>
+      <c r="D59" s="162"/>
+      <c r="E59" s="163" t="s">
+        <v>83</v>
+      </c>
+      <c r="F59" s="164"/>
+      <c r="G59" s="165"/>
+      <c r="H59" s="165"/>
+      <c r="I59" s="133"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="166" t="s">
         <v>84</v>
       </c>
-      <c r="C59" s="159"/>
-      <c r="D59" s="160"/>
-      <c r="E59" s="160" t="s">
-        <v>84</v>
-      </c>
-      <c r="F59" s="161"/>
-      <c r="G59" s="162"/>
-      <c r="H59" s="162"/>
-      <c r="I59" s="133"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="163" t="s">
+      <c r="B60" s="167" t="s">
         <v>85</v>
       </c>
-      <c r="B60" s="164" t="s">
+      <c r="C60" s="168"/>
+      <c r="D60" s="169"/>
+      <c r="E60" s="170"/>
+      <c r="F60" s="170"/>
+      <c r="G60" s="170" t="s">
         <v>86</v>
       </c>
-      <c r="C60" s="165"/>
-      <c r="D60" s="166"/>
-      <c r="E60" s="167"/>
-      <c r="F60" s="167"/>
-      <c r="G60" s="167" t="s">
+      <c r="H60" s="171"/>
+      <c r="I60" s="172"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="173"/>
+      <c r="B61" s="174" t="s">
         <v>87</v>
       </c>
-      <c r="H60" s="168"/>
-      <c r="I60" s="169"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="170"/>
-      <c r="B61" s="171" t="s">
+      <c r="C61" s="175"/>
+      <c r="D61" s="146"/>
+      <c r="E61" s="176"/>
+      <c r="F61" s="176"/>
+      <c r="G61" s="176" t="s">
         <v>88</v>
       </c>
-      <c r="C61" s="172"/>
-      <c r="D61" s="146"/>
-      <c r="E61" s="173"/>
-      <c r="F61" s="173"/>
-      <c r="G61" s="173" t="s">
+      <c r="H61" s="177"/>
+      <c r="I61" s="178"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="173"/>
+      <c r="B62" s="174" t="s">
         <v>89</v>
       </c>
-      <c r="H61" s="174"/>
-      <c r="I61" s="175"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="170"/>
-      <c r="B62" s="171" t="s">
+      <c r="C62" s="175"/>
+      <c r="D62" s="146"/>
+      <c r="E62" s="176"/>
+      <c r="F62" s="176"/>
+      <c r="G62" s="176" t="s">
         <v>90</v>
       </c>
-      <c r="C62" s="172"/>
-      <c r="D62" s="146"/>
-      <c r="E62" s="173"/>
-      <c r="F62" s="173"/>
-      <c r="G62" s="173" t="s">
+      <c r="H62" s="177"/>
+      <c r="I62" s="178"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="179"/>
+      <c r="B63" s="180" t="s">
         <v>91</v>
       </c>
-      <c r="H62" s="174"/>
-      <c r="I62" s="175"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="176"/>
-      <c r="B63" s="177" t="s">
+      <c r="C63" s="181"/>
+      <c r="D63" s="182"/>
+      <c r="E63" s="183"/>
+      <c r="F63" s="183"/>
+      <c r="G63" s="184" t="s">
         <v>92</v>
       </c>
-      <c r="C63" s="178"/>
-      <c r="D63" s="179"/>
-      <c r="E63" s="180"/>
-      <c r="F63" s="180"/>
-      <c r="G63" s="181" t="s">
+      <c r="H63" s="185"/>
+      <c r="I63" s="186"/>
+    </row>
+    <row r="64" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="187" t="s">
         <v>93</v>
       </c>
-      <c r="H63" s="182"/>
-      <c r="I63" s="183"/>
-    </row>
-    <row r="64" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="184" t="s">
+      <c r="B64" s="188" t="s">
         <v>94</v>
       </c>
-      <c r="B64" s="185" t="s">
+      <c r="C64" s="189"/>
+      <c r="D64" s="190"/>
+      <c r="E64" s="190"/>
+      <c r="F64" s="190"/>
+      <c r="G64" s="190"/>
+      <c r="H64" s="191"/>
+      <c r="I64" s="192"/>
+    </row>
+    <row r="65" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="193" t="s">
         <v>95</v>
       </c>
-      <c r="C64" s="186"/>
-      <c r="D64" s="187"/>
-      <c r="E64" s="187"/>
-      <c r="F64" s="187"/>
-      <c r="G64" s="187"/>
-      <c r="H64" s="186"/>
-      <c r="I64" s="188"/>
-    </row>
-    <row r="65" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="189" t="s">
+      <c r="B65" s="194" t="s">
         <v>96</v>
       </c>
-      <c r="B65" s="190" t="s">
+      <c r="C65" s="193" t="s">
         <v>97</v>
       </c>
-      <c r="C65" s="189" t="s">
+      <c r="D65" s="195" t="s">
         <v>98</v>
       </c>
-      <c r="D65" s="191" t="s">
+      <c r="E65" s="196"/>
+      <c r="F65" s="197" t="s">
         <v>99</v>
       </c>
-      <c r="E65" s="192"/>
-      <c r="F65" s="193" t="s">
+      <c r="G65" s="198"/>
+      <c r="H65" s="199" t="s">
         <v>100</v>
       </c>
-      <c r="G65" s="194"/>
-      <c r="H65" s="191" t="s">
+      <c r="I65" s="200" t="s">
         <v>101</v>
       </c>
-      <c r="I65" s="195" t="s">
+    </row>
+    <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="201" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="196" t="s">
+      <c r="B66" s="202"/>
+      <c r="C66" s="202"/>
+      <c r="D66" s="202"/>
+      <c r="E66" s="202"/>
+      <c r="F66" s="202"/>
+      <c r="G66" s="202"/>
+      <c r="H66" s="202"/>
+      <c r="I66" s="203"/>
+    </row>
+    <row r="67" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="204" t="s">
         <v>103</v>
       </c>
-      <c r="B66" s="197"/>
-      <c r="C66" s="197"/>
-      <c r="D66" s="197"/>
-      <c r="E66" s="197"/>
-      <c r="F66" s="197"/>
-      <c r="G66" s="197"/>
-      <c r="H66" s="197"/>
-      <c r="I66" s="198"/>
-    </row>
-    <row r="67" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="199" t="s">
+      <c r="B67" s="205" t="s">
         <v>104</v>
-      </c>
-      <c r="B67" s="200" t="s">
-        <v>105</v>
       </c>
       <c r="C67" s="141"/>
       <c r="D67" s="141" t="s">
+        <v>105</v>
+      </c>
+      <c r="E67" s="141"/>
+      <c r="F67" s="206"/>
+      <c r="G67" s="204" t="s">
         <v>106</v>
       </c>
-      <c r="E67" s="141"/>
-      <c r="F67" s="201"/>
-      <c r="G67" s="199" t="s">
+      <c r="H67" s="207" t="s">
         <v>107</v>
       </c>
-      <c r="H67" s="202" t="s">
+      <c r="I67" s="208"/>
+    </row>
+    <row r="68" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="209"/>
+      <c r="B68" s="210" t="s">
         <v>108</v>
-      </c>
-      <c r="I67" s="203"/>
-    </row>
-    <row r="68" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="204"/>
-      <c r="B68" s="205" t="s">
-        <v>109</v>
       </c>
       <c r="C68" s="149"/>
       <c r="D68" s="149" t="s">
+        <v>109</v>
+      </c>
+      <c r="E68" s="149"/>
+      <c r="F68" s="211"/>
+      <c r="G68" s="209"/>
+      <c r="H68" s="212"/>
+      <c r="I68" s="213"/>
+    </row>
+    <row r="69" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="214" t="s">
         <v>110</v>
       </c>
-      <c r="E68" s="149"/>
-      <c r="F68" s="206"/>
-      <c r="G68" s="204"/>
-      <c r="H68" s="207"/>
-      <c r="I68" s="208"/>
-    </row>
-    <row r="69" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="209" t="s">
+      <c r="B69" s="215" t="s">
         <v>111</v>
-      </c>
-      <c r="B69" s="210" t="s">
-        <v>112</v>
       </c>
       <c r="C69" s="141"/>
       <c r="D69" s="141"/>
       <c r="E69" s="141"/>
-      <c r="F69" s="211"/>
+      <c r="F69" s="216"/>
       <c r="G69" s="141"/>
       <c r="H69" s="141"/>
-      <c r="I69" s="201"/>
+      <c r="I69" s="206"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="212"/>
-      <c r="B70" s="213" t="s">
-        <v>113</v>
-      </c>
-      <c r="C70" s="162"/>
-      <c r="D70" s="162"/>
-      <c r="E70" s="162"/>
-      <c r="F70" s="162"/>
-      <c r="G70" s="162"/>
-      <c r="H70" s="162"/>
-      <c r="I70" s="214"/>
+      <c r="A70" s="217"/>
+      <c r="B70" s="218" t="s">
+        <v>112</v>
+      </c>
+      <c r="C70" s="165"/>
+      <c r="D70" s="165"/>
+      <c r="E70" s="165"/>
+      <c r="F70" s="165"/>
+      <c r="G70" s="165"/>
+      <c r="H70" s="165"/>
+      <c r="I70" s="219"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="137" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" s="220"/>
+      <c r="C71" s="221" t="s">
         <v>114</v>
       </c>
-      <c r="B71" s="215"/>
-      <c r="C71" s="216" t="s">
+      <c r="D71" s="222"/>
+      <c r="E71" s="223"/>
+      <c r="F71" s="224" t="s">
         <v>115</v>
       </c>
-      <c r="D71" s="217"/>
-      <c r="E71" s="218"/>
-      <c r="F71" s="219" t="s">
+      <c r="G71" s="225"/>
+      <c r="H71" s="226" t="s">
         <v>116</v>
       </c>
-      <c r="G71" s="220"/>
-      <c r="H71" s="221" t="s">
-        <v>117</v>
-      </c>
-      <c r="I71" s="221" t="s">
+      <c r="I71" s="226" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="144"/>
-      <c r="B72" s="222"/>
-      <c r="C72" s="223" t="s">
+      <c r="B72" s="227"/>
+      <c r="C72" s="228" t="s">
+        <v>117</v>
+      </c>
+      <c r="D72" s="221" t="s">
         <v>118</v>
       </c>
-      <c r="D72" s="216" t="s">
-        <v>119</v>
-      </c>
-      <c r="E72" s="218"/>
-      <c r="F72" s="224"/>
-      <c r="G72" s="225"/>
-      <c r="H72" s="226"/>
-      <c r="I72" s="226"/>
+      <c r="E72" s="223"/>
+      <c r="F72" s="229"/>
+      <c r="G72" s="230"/>
+      <c r="H72" s="231"/>
+      <c r="I72" s="231"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="144"/>
-      <c r="B73" s="227" t="s">
+      <c r="B73" s="232" t="s">
         <v>7</v>
       </c>
-      <c r="C73" s="228" t="s">
+      <c r="C73" s="233" t="s">
+        <v>119</v>
+      </c>
+      <c r="D73" s="234" t="s">
+        <v>119</v>
+      </c>
+      <c r="E73" s="235" t="s">
         <v>120</v>
       </c>
-      <c r="D73" s="229" t="s">
+      <c r="F73" s="234" t="s">
+        <v>119</v>
+      </c>
+      <c r="G73" s="235" t="s">
         <v>120</v>
       </c>
-      <c r="E73" s="230" t="s">
+      <c r="H73" s="233" t="s">
         <v>121</v>
       </c>
-      <c r="F73" s="229" t="s">
-        <v>120</v>
-      </c>
-      <c r="G73" s="230" t="s">
-        <v>121</v>
-      </c>
-      <c r="H73" s="228" t="s">
-        <v>122</v>
-      </c>
-      <c r="I73" s="228" t="s">
-        <v>120</v>
+      <c r="I73" s="233" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="144"/>
-      <c r="B74" s="231" t="s">
+      <c r="B74" s="236" t="s">
+        <v>122</v>
+      </c>
+      <c r="C74" s="237" t="s">
         <v>123</v>
       </c>
-      <c r="C74" s="232" t="s">
+      <c r="D74" s="238" t="s">
         <v>124</v>
       </c>
-      <c r="D74" s="233" t="s">
-        <v>125</v>
-      </c>
-      <c r="E74" s="234" t="s">
-        <v>124</v>
-      </c>
-      <c r="F74" s="235" t="s">
-        <v>124</v>
-      </c>
-      <c r="G74" s="234" t="s">
+      <c r="E74" s="239" t="s">
+        <v>123</v>
+      </c>
+      <c r="F74" s="240" t="s">
+        <v>123</v>
+      </c>
+      <c r="G74" s="239" t="s">
         <v>48</v>
       </c>
-      <c r="H74" s="232" t="s">
+      <c r="H74" s="237" t="s">
         <v>47</v>
       </c>
-      <c r="I74" s="232" t="s">
-        <v>124</v>
+      <c r="I74" s="237" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="144"/>
-      <c r="B75" s="236" t="s">
+      <c r="B75" s="241" t="s">
+        <v>125</v>
+      </c>
+      <c r="C75" s="242" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" s="243" t="s">
+        <v>123</v>
+      </c>
+      <c r="E75" s="244" t="s">
+        <v>48</v>
+      </c>
+      <c r="F75" s="245" t="s">
         <v>126</v>
       </c>
-      <c r="C75" s="237" t="s">
+      <c r="G75" s="244" t="s">
+        <v>127</v>
+      </c>
+      <c r="H75" s="242" t="s">
+        <v>47</v>
+      </c>
+      <c r="I75" s="242" t="s">
         <v>16</v>
       </c>
-      <c r="D75" s="238" t="s">
-        <v>124</v>
-      </c>
-      <c r="E75" s="239" t="s">
+    </row>
+    <row r="76" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="246"/>
+      <c r="B76" s="247" t="s">
+        <v>128</v>
+      </c>
+      <c r="C76" s="248" t="s">
+        <v>16</v>
+      </c>
+      <c r="D76" s="249" t="s">
+        <v>126</v>
+      </c>
+      <c r="E76" s="250" t="s">
+        <v>127</v>
+      </c>
+      <c r="F76" s="251" t="s">
         <v>48</v>
       </c>
-      <c r="F75" s="240" t="s">
-        <v>127</v>
-      </c>
-      <c r="G75" s="239" t="s">
-        <v>128</v>
-      </c>
-      <c r="H75" s="237" t="s">
+      <c r="G76" s="250" t="s">
         <v>47</v>
       </c>
-      <c r="I75" s="237" t="s">
+      <c r="H76" s="248" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="241"/>
-      <c r="B76" s="242" t="s">
-        <v>129</v>
-      </c>
-      <c r="C76" s="243" t="s">
-        <v>16</v>
-      </c>
-      <c r="D76" s="244" t="s">
-        <v>127</v>
-      </c>
-      <c r="E76" s="245" t="s">
-        <v>128</v>
-      </c>
-      <c r="F76" s="246" t="s">
-        <v>48</v>
-      </c>
-      <c r="G76" s="245" t="s">
-        <v>47</v>
-      </c>
-      <c r="H76" s="243" t="s">
-        <v>16</v>
-      </c>
-      <c r="I76" s="243" t="s">
+      <c r="I76" s="248" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4126,6 +4144,6 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.25" bottom="0.25" header="0.3" footer="0.05"/>
-  <pageSetup scale="62" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="61" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>